<commit_message>
dev update--trying out fft correlations
</commit_message>
<xml_diff>
--- a/docs/results.xlsx
+++ b/docs/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="27780" windowHeight="11070"/>
+    <workbookView xWindow="0" yWindow="330" windowWidth="28185" windowHeight="3000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
   <si>
     <t>-The sound is deep_growl_converted.wav @ 17 seconds.</t>
   </si>
@@ -65,6 +64,21 @@
   </si>
   <si>
     <t>match %</t>
+  </si>
+  <si>
+    <t>-these tests ran with fft correlation only</t>
+  </si>
+  <si>
+    <t>-using line in with minimum volume to trigger collection</t>
+  </si>
+  <si>
+    <t>-direct speaker connection with out using microphone and pre-amp</t>
+  </si>
+  <si>
+    <t>-comparison fft with microphone signal in soi[n]</t>
+  </si>
+  <si>
+    <t>-tests run with sounds on loop on vlc media player</t>
   </si>
 </sst>
 </file>
@@ -398,61 +412,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O139"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:15"/>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -466,7 +479,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -504,7 +517,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:12">
       <c r="A13" s="2">
         <v>41003</v>
       </c>
@@ -530,7 +543,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:12">
       <c r="A14" s="2">
         <v>41003</v>
       </c>
@@ -556,7 +569,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:12">
       <c r="A15" s="2">
         <v>41003</v>
       </c>
@@ -569,8 +582,10 @@
       <c r="F15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="G15" s="2"/>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="2">
         <v>41003</v>
       </c>
@@ -584,7 +599,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:14">
       <c r="A17" s="2">
         <v>41003</v>
       </c>
@@ -598,15 +613,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:14">
       <c r="A18" s="2">
         <v>41003</v>
       </c>
       <c r="C18">
         <v>92</v>
       </c>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="2">
         <v>41003</v>
       </c>
@@ -614,7 +630,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:14">
       <c r="A20" s="2">
         <v>41003</v>
       </c>
@@ -622,7 +638,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:14">
       <c r="A21" s="2">
         <v>41003</v>
       </c>
@@ -630,7 +646,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:14">
       <c r="A22" s="2">
         <v>41003</v>
       </c>
@@ -638,7 +654,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:14">
       <c r="A23" s="2">
         <v>41004</v>
       </c>
@@ -646,7 +662,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:14">
       <c r="A24" s="2">
         <v>41004</v>
       </c>
@@ -654,121 +670,197 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:15"/>
-    <row r="26" spans="1:15"/>
-    <row r="27" spans="1:15"/>
-    <row r="28" spans="1:15"/>
-    <row r="29" spans="1:15"/>
-    <row r="30" spans="1:15"/>
-    <row r="31" spans="1:15"/>
-    <row r="32" spans="1:15"/>
-    <row r="33" spans="1:1"/>
-    <row r="34" spans="1:1"/>
-    <row r="35" spans="1:1"/>
-    <row r="36" spans="1:1"/>
-    <row r="37" spans="1:1"/>
-    <row r="38" spans="1:1"/>
-    <row r="39" spans="1:1"/>
-    <row r="40" spans="1:1"/>
-    <row r="41" spans="1:1"/>
-    <row r="42" spans="1:1"/>
-    <row r="43" spans="1:1"/>
-    <row r="44" spans="1:1"/>
-    <row r="45" spans="1:1"/>
-    <row r="46" spans="1:1"/>
-    <row r="47" spans="1:1"/>
-    <row r="48" spans="1:1"/>
-    <row r="49" spans="1:1"/>
-    <row r="50" spans="1:1"/>
-    <row r="51" spans="1:1"/>
-    <row r="52" spans="1:1"/>
-    <row r="53" spans="1:1"/>
-    <row r="54" spans="1:1"/>
-    <row r="55" spans="1:1"/>
-    <row r="56" spans="1:1"/>
-    <row r="57" spans="1:1"/>
-    <row r="58" spans="1:1"/>
-    <row r="59" spans="1:1"/>
-    <row r="60" spans="1:1"/>
-    <row r="61" spans="1:1"/>
-    <row r="62" spans="1:1"/>
-    <row r="63" spans="1:1"/>
-    <row r="64" spans="1:1"/>
-    <row r="65" spans="1:1"/>
-    <row r="66" spans="1:1"/>
-    <row r="67" spans="1:1"/>
-    <row r="68" spans="1:1"/>
-    <row r="69" spans="1:1"/>
-    <row r="70" spans="1:1"/>
-    <row r="71" spans="1:1"/>
-    <row r="72" spans="1:1"/>
-    <row r="73" spans="1:1"/>
-    <row r="74" spans="1:1"/>
-    <row r="75" spans="1:1"/>
-    <row r="76" spans="1:1"/>
-    <row r="77" spans="1:1"/>
-    <row r="78" spans="1:1"/>
-    <row r="79" spans="1:1"/>
-    <row r="80" spans="1:1"/>
-    <row r="81" spans="1:1"/>
-    <row r="82" spans="1:1"/>
-    <row r="83" spans="1:1"/>
-    <row r="84" spans="1:1"/>
-    <row r="85" spans="1:1"/>
-    <row r="86" spans="1:1"/>
-    <row r="87" spans="1:1"/>
-    <row r="88" spans="1:1"/>
-    <row r="89" spans="1:1"/>
-    <row r="90" spans="1:1"/>
-    <row r="91" spans="1:1"/>
-    <row r="92" spans="1:1"/>
-    <row r="93" spans="1:1"/>
-    <row r="94" spans="1:1"/>
-    <row r="95" spans="1:1"/>
-    <row r="96" spans="1:1"/>
-    <row r="97" spans="1:1"/>
-    <row r="98" spans="1:1"/>
-    <row r="99" spans="1:1"/>
-    <row r="100" spans="1:1"/>
-    <row r="101" spans="1:1"/>
-    <row r="102" spans="1:1"/>
-    <row r="103" spans="1:1"/>
-    <row r="104" spans="1:1"/>
-    <row r="105" spans="1:1"/>
-    <row r="106" spans="1:1"/>
-    <row r="107" spans="1:1"/>
-    <row r="108" spans="1:1"/>
-    <row r="109" spans="1:1"/>
-    <row r="110" spans="1:1"/>
-    <row r="111" spans="1:1"/>
-    <row r="112" spans="1:1"/>
-    <row r="113" spans="1:1"/>
-    <row r="114" spans="1:1"/>
-    <row r="115" spans="1:1"/>
-    <row r="116" spans="1:1"/>
-    <row r="117" spans="1:1"/>
-    <row r="118" spans="1:1"/>
-    <row r="119" spans="1:1"/>
-    <row r="120" spans="1:1"/>
-    <row r="121" spans="1:1"/>
-    <row r="122" spans="1:1"/>
-    <row r="123" spans="1:1"/>
-    <row r="124" spans="1:1"/>
-    <row r="125" spans="1:1"/>
-    <row r="126" spans="1:1"/>
-    <row r="127" spans="1:1"/>
-    <row r="128" spans="1:1"/>
-    <row r="129" spans="1:1"/>
-    <row r="130" spans="1:1"/>
-    <row r="131" spans="1:1"/>
-    <row r="132" spans="1:1"/>
-    <row r="133" spans="1:1"/>
-    <row r="134" spans="1:1"/>
-    <row r="135" spans="1:1"/>
-    <row r="136" spans="1:1"/>
-    <row r="137" spans="1:1"/>
-    <row r="138" spans="1:1"/>
-    <row r="139" spans="1:1"/>
+    <row r="25" spans="1:14">
+      <c r="A25" s="2"/>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" t="s">
+        <v>15</v>
+      </c>
+      <c r="J29" t="s">
+        <v>13</v>
+      </c>
+      <c r="K29" t="s">
+        <v>14</v>
+      </c>
+      <c r="L29" t="s">
+        <v>15</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="2">
+        <v>41005</v>
+      </c>
+      <c r="C30">
+        <v>88</v>
+      </c>
+      <c r="D30" s="2">
+        <v>41005</v>
+      </c>
+      <c r="F30">
+        <v>37</v>
+      </c>
+      <c r="G30" s="2">
+        <v>41005</v>
+      </c>
+      <c r="I30">
+        <v>34</v>
+      </c>
+      <c r="J30" s="2">
+        <v>41005</v>
+      </c>
+      <c r="L30">
+        <v>11</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="2">
+        <v>41005</v>
+      </c>
+      <c r="C31">
+        <v>79</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="N31" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="2">
+        <v>41005</v>
+      </c>
+      <c r="C32">
+        <v>68</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="N32" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" s="2">
+        <v>41005</v>
+      </c>
+      <c r="C33">
+        <v>89</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="N33" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" s="2">
+        <v>41005</v>
+      </c>
+      <c r="C34">
+        <v>91</v>
+      </c>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" s="2">
+        <v>41005</v>
+      </c>
+      <c r="C35">
+        <v>56</v>
+      </c>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" s="2">
+        <v>41005</v>
+      </c>
+      <c r="C36">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="2">
+        <v>41005</v>
+      </c>
+      <c r="C37">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" s="2">
+        <v>41005</v>
+      </c>
+      <c r="C38">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" s="2">
+        <v>41005</v>
+      </c>
+      <c r="C39">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" s="2">
+        <v>41005</v>
+      </c>
+      <c r="C40">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dev update--almost ready to merge back to the head
</commit_message>
<xml_diff>
--- a/docs/results.xlsx
+++ b/docs/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="23">
   <si>
     <t>-The sound is deep_growl_converted.wav @ 17 seconds.</t>
   </si>
@@ -69,16 +69,22 @@
     <t>-these tests ran with fft correlation only</t>
   </si>
   <si>
-    <t>-using line in with minimum volume to trigger collection</t>
-  </si>
-  <si>
     <t>-direct speaker connection with out using microphone and pre-amp</t>
   </si>
   <si>
     <t>-comparison fft with microphone signal in soi[n]</t>
   </si>
   <si>
-    <t>-tests run with sounds on loop on vlc media player</t>
+    <t>-using line in with minimum volume to trigger collection, 3 dB gain on line input</t>
+  </si>
+  <si>
+    <t>-using new reset algorithm to avoid stopping and starting dsk</t>
+  </si>
+  <si>
+    <t>-tests run with sounds on loop on vlc media player--pseudo random</t>
+  </si>
+  <si>
+    <t>-set decision at 55 and you're wrong 16% of the time</t>
   </si>
 </sst>
 </file>
@@ -412,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N41"/>
+  <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -757,7 +763,7 @@
         <v>11</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:14">
@@ -768,10 +774,23 @@
         <v>79</v>
       </c>
       <c r="D31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="J31" s="2"/>
+      <c r="F31">
+        <v>53</v>
+      </c>
+      <c r="G31" s="2">
+        <v>41005</v>
+      </c>
+      <c r="I31">
+        <v>8</v>
+      </c>
+      <c r="J31" s="2">
+        <v>41005</v>
+      </c>
+      <c r="L31">
+        <v>9</v>
+      </c>
       <c r="N31" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:14">
@@ -782,10 +801,23 @@
         <v>68</v>
       </c>
       <c r="D32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="J32" s="2"/>
+      <c r="F32">
+        <v>58</v>
+      </c>
+      <c r="G32" s="2">
+        <v>41005</v>
+      </c>
+      <c r="I32">
+        <v>29</v>
+      </c>
+      <c r="J32" s="2">
+        <v>41005</v>
+      </c>
+      <c r="L32">
+        <v>13</v>
+      </c>
       <c r="N32" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:14">
@@ -796,8 +828,23 @@
         <v>89</v>
       </c>
       <c r="D33" s="2"/>
+      <c r="F33">
+        <v>58</v>
+      </c>
+      <c r="G33" s="2">
+        <v>41005</v>
+      </c>
+      <c r="I33">
+        <v>11</v>
+      </c>
+      <c r="J33" s="2">
+        <v>41005</v>
+      </c>
+      <c r="L33">
+        <v>13</v>
+      </c>
       <c r="N33" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:14">
@@ -808,6 +855,24 @@
         <v>91</v>
       </c>
       <c r="D34" s="2"/>
+      <c r="F34">
+        <v>59</v>
+      </c>
+      <c r="G34" s="2">
+        <v>41005</v>
+      </c>
+      <c r="I34">
+        <v>12</v>
+      </c>
+      <c r="J34" s="2">
+        <v>41005</v>
+      </c>
+      <c r="L34">
+        <v>14</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="35" spans="1:14">
       <c r="A35" s="2">
@@ -817,6 +882,21 @@
         <v>56</v>
       </c>
       <c r="D35" s="2"/>
+      <c r="F35">
+        <v>52</v>
+      </c>
+      <c r="G35" s="2">
+        <v>41005</v>
+      </c>
+      <c r="I35">
+        <v>38</v>
+      </c>
+      <c r="J35" s="2">
+        <v>41005</v>
+      </c>
+      <c r="L35">
+        <v>16</v>
+      </c>
     </row>
     <row r="36" spans="1:14">
       <c r="A36" s="2">
@@ -825,6 +905,21 @@
       <c r="C36">
         <v>67</v>
       </c>
+      <c r="F36">
+        <v>58</v>
+      </c>
+      <c r="G36" s="2">
+        <v>41005</v>
+      </c>
+      <c r="I36">
+        <v>40</v>
+      </c>
+      <c r="J36" s="2">
+        <v>41005</v>
+      </c>
+      <c r="L36">
+        <v>15</v>
+      </c>
     </row>
     <row r="37" spans="1:14">
       <c r="A37" s="2">
@@ -833,6 +928,21 @@
       <c r="C37">
         <v>45</v>
       </c>
+      <c r="F37">
+        <v>59</v>
+      </c>
+      <c r="G37" s="2">
+        <v>41005</v>
+      </c>
+      <c r="I37">
+        <v>24</v>
+      </c>
+      <c r="J37" s="2">
+        <v>41005</v>
+      </c>
+      <c r="L37">
+        <v>17</v>
+      </c>
     </row>
     <row r="38" spans="1:14">
       <c r="A38" s="2">
@@ -841,6 +951,21 @@
       <c r="C38">
         <v>79</v>
       </c>
+      <c r="F38">
+        <v>50</v>
+      </c>
+      <c r="G38" s="2">
+        <v>41005</v>
+      </c>
+      <c r="I38">
+        <v>12</v>
+      </c>
+      <c r="J38" s="2">
+        <v>41005</v>
+      </c>
+      <c r="L38">
+        <v>18</v>
+      </c>
     </row>
     <row r="39" spans="1:14">
       <c r="A39" s="2">
@@ -849,6 +974,21 @@
       <c r="C39">
         <v>50</v>
       </c>
+      <c r="F39">
+        <v>32</v>
+      </c>
+      <c r="G39" s="2">
+        <v>41005</v>
+      </c>
+      <c r="I39">
+        <v>39</v>
+      </c>
+      <c r="J39" s="2">
+        <v>41005</v>
+      </c>
+      <c r="L39">
+        <v>9</v>
+      </c>
     </row>
     <row r="40" spans="1:14">
       <c r="A40" s="2">
@@ -857,9 +997,206 @@
       <c r="C40">
         <v>89</v>
       </c>
+      <c r="F40">
+        <v>27</v>
+      </c>
+      <c r="G40" s="2">
+        <v>41005</v>
+      </c>
+      <c r="I40">
+        <v>9</v>
+      </c>
+      <c r="J40" s="2">
+        <v>41005</v>
+      </c>
+      <c r="L40">
+        <v>15</v>
+      </c>
     </row>
     <row r="41" spans="1:14">
-      <c r="A41" s="2"/>
+      <c r="A41" s="2">
+        <v>41005</v>
+      </c>
+      <c r="C41">
+        <v>62</v>
+      </c>
+      <c r="F41">
+        <v>60</v>
+      </c>
+      <c r="G41" s="2">
+        <v>41005</v>
+      </c>
+      <c r="I41">
+        <v>12</v>
+      </c>
+      <c r="J41" s="2">
+        <v>41005</v>
+      </c>
+      <c r="L41">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="C42">
+        <f>AVERAGE(C31:C41)</f>
+        <v>70.454545454545453</v>
+      </c>
+      <c r="F42">
+        <f>AVERAGE(F31:F41)</f>
+        <v>51.454545454545453</v>
+      </c>
+      <c r="I42">
+        <f>AVERAGE(I31:I41)</f>
+        <v>21.272727272727273</v>
+      </c>
+      <c r="L42">
+        <f>AVERAGE(L31:L41)</f>
+        <v>13.636363636363637</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="C43">
+        <f>STDEV(C30:C41)</f>
+        <v>16.245045864863386</v>
+      </c>
+      <c r="F43">
+        <f>STDEV(F30:F41)</f>
+        <v>11.631657428993279</v>
+      </c>
+      <c r="I43">
+        <f>STDEV(I30:I41)</f>
+        <v>12.970829743791423</v>
+      </c>
+      <c r="L43">
+        <f>STDEV(L30:L41)</f>
+        <v>2.9682665076785213</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="C44" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" t="s">
+        <v>10</v>
+      </c>
+      <c r="G46" t="s">
+        <v>11</v>
+      </c>
+      <c r="J46" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F47" t="s">
+        <v>15</v>
+      </c>
+      <c r="G47" t="s">
+        <v>13</v>
+      </c>
+      <c r="H47" t="s">
+        <v>14</v>
+      </c>
+      <c r="I47" t="s">
+        <v>15</v>
+      </c>
+      <c r="J47" t="s">
+        <v>13</v>
+      </c>
+      <c r="K47" t="s">
+        <v>14</v>
+      </c>
+      <c r="L47" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="J48" s="2"/>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="J49" s="2"/>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="J50" s="2"/>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="J51" s="2"/>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="J52" s="2"/>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="J53" s="2"/>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="J54" s="2"/>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="J55" s="2"/>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="J56" s="2"/>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="J57" s="2"/>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="J58" s="2"/>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="J59" s="2"/>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="C62" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>